<commit_message>
Finished processing aakash study. Found YPs.
</commit_message>
<xml_diff>
--- a/example/info/02 foot corrected info.xlsx
+++ b/example/info/02 foot corrected info.xlsx
@@ -566,13 +566,13 @@
         <v>0.002486644345176593</v>
       </c>
       <c r="M2" t="n">
-        <v>158.4063909161324</v>
+        <v>158.406047302999</v>
       </c>
       <c r="N2" t="n">
         <v>0.001167465321559093</v>
       </c>
       <c r="O2" t="n">
-        <v>74.3710783385158</v>
+        <v>74.37073472538241</v>
       </c>
       <c r="P2" t="n">
         <v>63702.73562050127</v>
@@ -631,13 +631,13 @@
         <v>0.003652802999034743</v>
       </c>
       <c r="M3" t="n">
-        <v>198.5134716935894</v>
+        <v>198.512982112349</v>
       </c>
       <c r="N3" t="n">
         <v>0.001348872139951843</v>
       </c>
       <c r="O3" t="n">
-        <v>73.30546416127233</v>
+        <v>73.3049745800319</v>
       </c>
       <c r="P3" t="n">
         <v>54345.38412413871</v>
@@ -696,13 +696,13 @@
         <v>0.001771310291409529</v>
       </c>
       <c r="M4" t="n">
-        <v>115.5909349434113</v>
+        <v>115.590404178709</v>
       </c>
       <c r="N4" t="n">
         <v>0.000558242918370003</v>
       </c>
       <c r="O4" t="n">
-        <v>36.42979156515903</v>
+        <v>36.4292608004567</v>
       </c>
       <c r="P4" t="n">
         <v>65257.0047943025</v>
@@ -757,13 +757,13 @@
         <v>0.003234063939585186</v>
       </c>
       <c r="M5" t="n">
-        <v>192.9471588276287</v>
+        <v>192.947593520996</v>
       </c>
       <c r="N5" t="n">
         <v>0.0005903185807671863</v>
       </c>
       <c r="O5" t="n">
-        <v>35.21858128699316</v>
+        <v>35.2190159803605</v>
       </c>
       <c r="P5" t="n">
         <v>59661.03241166723</v>
@@ -818,13 +818,13 @@
         <v>0.00381451361088899</v>
       </c>
       <c r="M6" t="n">
-        <v>212.4615012161644</v>
+        <v>212.461144507981</v>
       </c>
       <c r="N6" t="n">
         <v>0.0002194805336283904</v>
       </c>
       <c r="O6" t="n">
-        <v>12.225004495203</v>
+        <v>12.2246477870196</v>
       </c>
       <c r="P6" t="n">
         <v>55698.09579430651</v>
@@ -879,13 +879,13 @@
         <v>0.001422674189591884</v>
       </c>
       <c r="M7" t="n">
-        <v>100.1160977889457</v>
+        <v>100.116005949159</v>
       </c>
       <c r="N7" t="n">
         <v>0.0005565689981795843</v>
       </c>
       <c r="O7" t="n">
-        <v>39.16680024042854</v>
+        <v>39.1667084006418</v>
       </c>
       <c r="P7" t="n">
         <v>70371.70329060289</v>
@@ -940,13 +940,13 @@
         <v>0.00215681772142884</v>
       </c>
       <c r="M8" t="n">
-        <v>133.4847491774616</v>
+        <v>133.484577967839</v>
       </c>
       <c r="N8" t="n">
         <v>0.0008960826996215404</v>
       </c>
       <c r="O8" t="n">
-        <v>55.45836769737319</v>
+        <v>55.4581964877506</v>
       </c>
       <c r="P8" t="n">
         <v>61889.59625174473</v>
@@ -1001,13 +1001,13 @@
         <v>0.002644136638289646</v>
       </c>
       <c r="M9" t="n">
-        <v>153.0248295440713</v>
+        <v>153.024416048495</v>
       </c>
       <c r="N9" t="n">
         <v>0.002418187927348046</v>
       </c>
       <c r="O9" t="n">
-        <v>139.9484744692012</v>
+        <v>139.948060973625</v>
       </c>
       <c r="P9" t="n">
         <v>57873.11208980431</v>
@@ -1062,13 +1062,13 @@
         <v>0.003383981439116137</v>
       </c>
       <c r="M10" t="n">
-        <v>183.5635998885492</v>
+        <v>183.56403158262</v>
       </c>
       <c r="N10" t="n">
         <v>0.0005319670038823366</v>
       </c>
       <c r="O10" t="n">
-        <v>28.85611189473629</v>
+        <v>28.8565435888071</v>
       </c>
       <c r="P10" t="n">
         <v>54244.98771203815</v>
@@ -1123,13 +1123,13 @@
         <v>0.003408700883743779</v>
       </c>
       <c r="M11" t="n">
-        <v>186.0033510010273</v>
+        <v>186.003104711952</v>
       </c>
       <c r="N11" t="n">
         <v>0.001751694515012279</v>
       </c>
       <c r="O11" t="n">
-        <v>95.58522995632265</v>
+        <v>95.5849836672474</v>
       </c>
       <c r="P11" t="n">
         <v>54567.15360359359</v>
@@ -1184,13 +1184,13 @@
         <v>0.003768694015879434</v>
       </c>
       <c r="M12" t="n">
-        <v>197.8245950881387</v>
+        <v>197.823708886257</v>
       </c>
       <c r="N12" t="n">
         <v>0.003001317510089134</v>
       </c>
       <c r="O12" t="n">
-        <v>157.5439923520237</v>
+        <v>157.543106150142</v>
       </c>
       <c r="P12" t="n">
         <v>52491.31610386107</v>
@@ -1245,13 +1245,13 @@
         <v>0.002831397119518019</v>
       </c>
       <c r="M13" t="n">
-        <v>164.6106155871639</v>
+        <v>164.610840241371</v>
       </c>
       <c r="N13" t="n">
         <v>0.002369830775605819</v>
       </c>
       <c r="O13" t="n">
-        <v>137.776222356073</v>
+        <v>137.77644701028</v>
       </c>
       <c r="P13" t="n">
         <v>58137.67313198094</v>
@@ -1306,13 +1306,13 @@
         <v>0.003337599360594599</v>
       </c>
       <c r="M14" t="n">
-        <v>191.9331133055703</v>
+        <v>191.93280380166</v>
       </c>
       <c r="N14" t="n">
         <v>0.001092961678286598</v>
       </c>
       <c r="O14" t="n">
-        <v>62.85243065362881</v>
+        <v>62.8521211497185</v>
       </c>
       <c r="P14" t="n">
         <v>57506.24417888996</v>
@@ -1367,13 +1367,13 @@
         <v>0.003052171734517982</v>
       </c>
       <c r="M15" t="n">
-        <v>179.0136807905835</v>
+        <v>179.013564063243</v>
       </c>
       <c r="N15" t="n">
         <v>0.0007991534053124824</v>
       </c>
       <c r="O15" t="n">
-        <v>46.87143058571933</v>
+        <v>46.8713138583788</v>
       </c>
       <c r="P15" t="n">
         <v>58651.20957602798</v>
@@ -1428,13 +1428,13 @@
         <v>0.0007660653984972492</v>
       </c>
       <c r="M16" t="n">
-        <v>56.3770243526542</v>
+        <v>56.3769290357358</v>
       </c>
       <c r="N16" t="n">
         <v>0.0004235744015886492</v>
       </c>
       <c r="O16" t="n">
-        <v>31.1721388872994</v>
+        <v>31.172043570381</v>
       </c>
       <c r="P16" t="n">
         <v>73592.84095891487</v>
@@ -1489,13 +1489,13 @@
         <v>0.002407070069901566</v>
       </c>
       <c r="M17" t="n">
-        <v>144.2476107123307</v>
+        <v>144.247777516109</v>
       </c>
       <c r="N17" t="n">
         <v>0.0006398491389772658</v>
       </c>
       <c r="O17" t="n">
-        <v>38.34388366536361</v>
+        <v>38.3440504691419</v>
       </c>
       <c r="P17" t="n">
         <v>59926.70480174591</v>
@@ -1550,13 +1550,13 @@
         <v>0.004564315429236116</v>
       </c>
       <c r="M18" t="n">
-        <v>227.601982530018</v>
+        <v>227.601528876447</v>
       </c>
       <c r="N18" t="n">
         <v>0.001575554387021716</v>
       </c>
       <c r="O18" t="n">
-        <v>78.56614282947243</v>
+        <v>78.5656891759014</v>
       </c>
       <c r="P18" t="n">
         <v>49865.42503582808</v>
@@ -1611,13 +1611,13 @@
         <v>0.001810033408109702</v>
       </c>
       <c r="M19" t="n">
-        <v>102.2348148797844</v>
+        <v>102.235369819713</v>
       </c>
       <c r="N19" t="n">
         <v>0.0006185604438029022</v>
       </c>
       <c r="O19" t="n">
-        <v>34.93733926948187</v>
+        <v>34.9378942094105</v>
       </c>
       <c r="P19" t="n">
         <v>56482.58720621179</v>
@@ -1672,13 +1672,13 @@
         <v>0.002946729411013637</v>
       </c>
       <c r="M20" t="n">
-        <v>203.7238741583147</v>
+        <v>203.724300085789</v>
       </c>
       <c r="N20" t="n">
         <v>0.001213498041939837</v>
       </c>
       <c r="O20" t="n">
-        <v>83.89565164438143</v>
+        <v>83.8960775718557</v>
       </c>
       <c r="P20" t="n">
         <v>69135.73378144363</v>
@@ -1733,13 +1733,13 @@
         <v>0.003099591938447006</v>
       </c>
       <c r="M21" t="n">
-        <v>184.9622728844121</v>
+        <v>184.962353082935</v>
       </c>
       <c r="N21" t="n">
         <v>9.850138957700637e-05</v>
       </c>
       <c r="O21" t="n">
-        <v>5.877806039376653</v>
+        <v>5.87788623789952</v>
       </c>
       <c r="P21" t="n">
         <v>59673.13012680211</v>
@@ -1794,13 +1794,13 @@
         <v>0.002538236159027514</v>
       </c>
       <c r="M22" t="n">
-        <v>147.6501358560565</v>
+        <v>147.650044884146</v>
       </c>
       <c r="N22" t="n">
         <v>0.0008695210452605134</v>
       </c>
       <c r="O22" t="n">
-        <v>50.58042050657961</v>
+        <v>50.5803295346691</v>
       </c>
       <c r="P22" t="n">
         <v>58170.33389860614</v>
@@ -1855,13 +1855,13 @@
         <v>0.002986865689476005</v>
       </c>
       <c r="M23" t="n">
-        <v>176.9798684822098</v>
+        <v>176.979439785403</v>
       </c>
       <c r="N23" t="n">
         <v>0.001295917891209504</v>
       </c>
       <c r="O23" t="n">
-        <v>76.78688186818282</v>
+        <v>76.786453171376</v>
       </c>
       <c r="P23" t="n">
         <v>59252.56043784516</v>
@@ -1916,13 +1916,13 @@
         <v>0.002913928760891397</v>
       </c>
       <c r="M24" t="n">
-        <v>164.5283642159548</v>
+        <v>164.528068453978</v>
       </c>
       <c r="N24" t="n">
         <v>0.0002542523812495404</v>
       </c>
       <c r="O24" t="n">
-        <v>14.35605275516236</v>
+        <v>14.3557569931856</v>
       </c>
       <c r="P24" t="n">
         <v>56462.62553228906</v>
@@ -1977,13 +1977,13 @@
         <v>0.002799291831076681</v>
       </c>
       <c r="M25" t="n">
-        <v>166.1483021730769</v>
+        <v>166.148394269309</v>
       </c>
       <c r="N25" t="n">
         <v>9.348677992880878e-06</v>
       </c>
       <c r="O25" t="n">
-        <v>0.5547867555596939</v>
+        <v>0.554878851791746</v>
       </c>
       <c r="P25" t="n">
         <v>59353.72383286097</v>
@@ -2038,13 +2038,13 @@
         <v>0.002342094147758236</v>
       </c>
       <c r="M26" t="n">
-        <v>143.2646318769509</v>
+        <v>143.264709458966</v>
       </c>
       <c r="N26" t="n">
         <v>6.561829182213629e-05</v>
       </c>
       <c r="O26" t="n">
-        <v>4.013760000940314</v>
+        <v>4.01383758295543</v>
       </c>
       <c r="P26" t="n">
         <v>61169.49209582098</v>
@@ -2099,13 +2099,13 @@
         <v>0.001877897583312018</v>
       </c>
       <c r="M27" t="n">
-        <v>114.9455756842076</v>
+        <v>114.945593796641</v>
       </c>
       <c r="N27" t="n">
         <v>4.202040312191429e-05</v>
       </c>
       <c r="O27" t="n">
-        <v>2.572039187892832</v>
+        <v>2.57205730032622</v>
       </c>
       <c r="P27" t="n">
         <v>61209.7245441433</v>
@@ -2160,13 +2160,13 @@
         <v>0.003608067645741652</v>
       </c>
       <c r="M28" t="n">
-        <v>211.2816199918306</v>
+        <v>211.28186215837</v>
       </c>
       <c r="N28" t="n">
         <v>0.0003993781755485524</v>
       </c>
       <c r="O28" t="n">
-        <v>23.38661554243398</v>
+        <v>23.3868577089734</v>
       </c>
       <c r="P28" t="n">
         <v>58558.17653744132</v>
@@ -2221,13 +2221,13 @@
         <v>0.001648224949389607</v>
       </c>
       <c r="M29" t="n">
-        <v>100.821098846987</v>
+        <v>100.820663952542</v>
       </c>
       <c r="N29" t="n">
         <v>0.000420692461308671</v>
       </c>
       <c r="O29" t="n">
-        <v>25.73387212015672</v>
+        <v>25.7334372257117</v>
       </c>
       <c r="P29" t="n">
         <v>61169.23784576812</v>
@@ -2282,13 +2282,13 @@
         <v>0.001742321762701669</v>
       </c>
       <c r="M30" t="n">
-        <v>117.0193528091357</v>
+        <v>117.019256302744</v>
       </c>
       <c r="N30" t="n">
         <v>0.0006749432958574685</v>
       </c>
       <c r="O30" t="n">
-        <v>45.33119677646712</v>
+        <v>45.3311002700754</v>
       </c>
       <c r="P30" t="n">
         <v>67162.82767500551</v>
@@ -2343,13 +2343,13 @@
         <v>0.003770420637788741</v>
       </c>
       <c r="M31" t="n">
-        <v>185.924558513989</v>
+        <v>185.923507771131</v>
       </c>
       <c r="N31" t="n">
         <v>0.001201807354363141</v>
       </c>
       <c r="O31" t="n">
-        <v>59.26346744747858</v>
+        <v>59.2624167046206</v>
       </c>
       <c r="P31" t="n">
         <v>49311.07842656266</v>
@@ -2404,13 +2404,13 @@
         <v>0.000542026924884292</v>
       </c>
       <c r="M32" t="n">
-        <v>46.12722918931409</v>
+        <v>46.1272742639521</v>
       </c>
       <c r="N32" t="n">
         <v>4.254760559954508e-05</v>
       </c>
       <c r="O32" t="n">
-        <v>3.620817621774421</v>
+        <v>3.62086269641244</v>
       </c>
       <c r="P32" t="n">
         <v>85101.44449705892</v>
@@ -2465,13 +2465,13 @@
         <v>0.003575680588424118</v>
       </c>
       <c r="M33" t="n">
-        <v>193.3422308899405</v>
+        <v>193.34158337017</v>
       </c>
       <c r="N33" t="n">
         <v>0.001764194556589218</v>
       </c>
       <c r="O33" t="n">
-        <v>95.39288418885208</v>
+        <v>95.3922366690816</v>
       </c>
       <c r="P33" t="n">
         <v>54071.26799750867</v>
@@ -2526,13 +2526,13 @@
         <v>0.0005830672385619013</v>
       </c>
       <c r="M34" t="n">
-        <v>44.36083542326781</v>
+        <v>44.360833762824</v>
       </c>
       <c r="N34" t="n">
         <v>0.0001722150993256013</v>
       </c>
       <c r="O34" t="n">
-        <v>13.10244489061711</v>
+        <v>13.1024432301733</v>
       </c>
       <c r="P34" t="n">
         <v>76081.84927734443</v>
@@ -2587,13 +2587,13 @@
         <v>0.0007326478168975564</v>
       </c>
       <c r="M35" t="n">
-        <v>48.18335937192787</v>
+        <v>48.1833180137349</v>
       </c>
       <c r="N35" t="n">
         <v>0.0004947773424867565</v>
       </c>
       <c r="O35" t="n">
-        <v>32.53956920389388</v>
+        <v>32.5395278457009</v>
       </c>
       <c r="P35" t="n">
         <v>65766.00230349448</v>
@@ -2648,13 +2648,13 @@
         <v>0.002594532464993202</v>
       </c>
       <c r="M36" t="n">
-        <v>144.0264646308588</v>
+        <v>144.025333226662</v>
       </c>
       <c r="N36" t="n">
         <v>0.0007298762958923019</v>
       </c>
       <c r="O36" t="n">
-        <v>40.51736242017908</v>
+        <v>40.5162310159823</v>
       </c>
       <c r="P36" t="n">
         <v>55511.09310441385</v>
@@ -2709,13 +2709,13 @@
         <v>0.004883037301830246</v>
       </c>
       <c r="M37" t="n">
-        <v>218.9485800295701</v>
+        <v>218.94767432926</v>
       </c>
       <c r="N37" t="n">
         <v>0.002233950269629646</v>
       </c>
       <c r="O37" t="n">
-        <v>100.1677047373161</v>
+        <v>100.166799037006</v>
       </c>
       <c r="P37" t="n">
         <v>44838.41936804264</v>
@@ -2770,13 +2770,13 @@
         <v>0.003201193006741849</v>
       </c>
       <c r="M38" t="n">
-        <v>174.5820286655862</v>
+        <v>174.581165598501</v>
       </c>
       <c r="N38" t="n">
         <v>0.0005973992805999486</v>
       </c>
       <c r="O38" t="n">
-        <v>32.58079889575783</v>
+        <v>32.5799358286726</v>
       </c>
       <c r="P38" t="n">
         <v>54536.28232687803</v>
@@ -2831,13 +2831,13 @@
         <v>0.003535944426428289</v>
       </c>
       <c r="M39" t="n">
-        <v>176.3048854168081</v>
+        <v>176.304083740973</v>
       </c>
       <c r="N39" t="n">
         <v>0.001604180994517588</v>
       </c>
       <c r="O39" t="n">
-        <v>79.98612561905968</v>
+        <v>79.9853239432246</v>
       </c>
       <c r="P39" t="n">
         <v>49860.53582269121</v>
@@ -2892,13 +2892,13 @@
         <v>0.002197614221644402</v>
       </c>
       <c r="M40" t="n">
-        <v>126.3279354864686</v>
+        <v>126.327924989666</v>
       </c>
       <c r="N40" t="n">
         <v>0.0003662964402999018</v>
       </c>
       <c r="O40" t="n">
-        <v>21.05623991980061</v>
+        <v>21.056229422998</v>
       </c>
       <c r="P40" t="n">
         <v>57484.122438532</v>
@@ -2953,13 +2953,13 @@
         <v>0.002440386540067831</v>
       </c>
       <c r="M41" t="n">
-        <v>127.1423105188142</v>
+        <v>127.142187354785</v>
       </c>
       <c r="N41" t="n">
         <v>0.001272923963641631</v>
       </c>
       <c r="O41" t="n">
-        <v>66.31844381384781</v>
+        <v>66.3183206498186</v>
       </c>
       <c r="P41" t="n">
         <v>52099.20037964602</v>
@@ -3014,13 +3014,13 @@
         <v>0.002919619240649738</v>
       </c>
       <c r="M42" t="n">
-        <v>137.9158431015865</v>
+        <v>137.914967289347</v>
       </c>
       <c r="N42" t="n">
         <v>0.0004717993448001379</v>
       </c>
       <c r="O42" t="n">
-        <v>22.28740903523806</v>
+        <v>22.2865332229986</v>
       </c>
       <c r="P42" t="n">
         <v>47237.31278694243</v>
@@ -3075,13 +3075,13 @@
         <v>0.0007756972094795218</v>
       </c>
       <c r="M43" t="n">
-        <v>43.69108441394191</v>
+        <v>43.69035133474</v>
       </c>
       <c r="N43" t="n">
         <v>0.0004853675214597392</v>
       </c>
       <c r="O43" t="n">
-        <v>27.3385619122806</v>
+        <v>27.3378288330787</v>
       </c>
       <c r="P43" t="n">
         <v>56323.97641865361</v>
@@ -3136,13 +3136,13 @@
         <v>0.004385461460634597</v>
       </c>
       <c r="M44" t="n">
-        <v>190.8077392575526</v>
+        <v>190.806708666229</v>
       </c>
       <c r="N44" t="n">
         <v>0.002048999318419596</v>
       </c>
       <c r="O44" t="n">
-        <v>89.15078587167571</v>
+        <v>89.1497552803521</v>
       </c>
       <c r="P44" t="n">
         <v>43508.92383366616</v>
@@ -3197,13 +3197,13 @@
         <v>0.002229400711533884</v>
       </c>
       <c r="M45" t="n">
-        <v>106.4245148630678</v>
+        <v>106.423782753718</v>
       </c>
       <c r="N45" t="n">
         <v>0.001046438241381984</v>
       </c>
       <c r="O45" t="n">
-        <v>49.95402919491335</v>
+        <v>49.9532970855636</v>
       </c>
       <c r="P45" t="n">
         <v>47736.49806565988</v>
@@ -3258,13 +3258,13 @@
         <v>0.001642667931312869</v>
       </c>
       <c r="M46" t="n">
-        <v>86.96944812573788</v>
+        <v>86.96884979516319</v>
       </c>
       <c r="N46" t="n">
         <v>0.0008846657864568686</v>
       </c>
       <c r="O46" t="n">
-        <v>46.83804151350449</v>
+        <v>46.8374431829298</v>
       </c>
       <c r="P46" t="n">
         <v>52943.65838484174</v>
@@ -3319,13 +3319,13 @@
         <v>0.002029688456395919</v>
       </c>
       <c r="M47" t="n">
-        <v>98.31398853798423</v>
+        <v>98.3135045128474</v>
       </c>
       <c r="N47" t="n">
         <v>0.0002692857965243188</v>
       </c>
       <c r="O47" t="n">
-        <v>13.04407713836243</v>
+        <v>13.0435931132256</v>
       </c>
       <c r="P47" t="n">
         <v>48437.73151640273</v>
@@ -3384,13 +3384,13 @@
         <v>0.002063402786403701</v>
       </c>
       <c r="M48" t="n">
-        <v>107.5314071020491</v>
+        <v>107.531322495733</v>
       </c>
       <c r="N48" t="n">
         <v>0.0004515525620684005</v>
       </c>
       <c r="O48" t="n">
-        <v>23.53210874406575</v>
+        <v>23.5320241377496</v>
       </c>
       <c r="P48" t="n">
         <v>52113.58790648386</v>
@@ -3445,13 +3445,13 @@
         <v>0.004696947534094185</v>
       </c>
       <c r="M49" t="n">
-        <v>214.623546449757</v>
+        <v>214.622689722153</v>
       </c>
       <c r="N49" t="n">
         <v>0.001324219784092684</v>
       </c>
       <c r="O49" t="n">
-        <v>60.50985960282357</v>
+        <v>60.5090028752196</v>
       </c>
       <c r="P49" t="n">
         <v>45694.07858279248</v>
@@ -3506,13 +3506,13 @@
         <v>0.002872619939431664</v>
       </c>
       <c r="M50" t="n">
-        <v>151.7381014629126</v>
+        <v>151.737831510864</v>
       </c>
       <c r="N50" t="n">
         <v>0.0005664390169995643</v>
       </c>
       <c r="O50" t="n">
-        <v>29.92077107468028</v>
+        <v>29.9205011226317</v>
       </c>
       <c r="P50" t="n">
         <v>52822.10480683522</v>
@@ -3571,13 +3571,13 @@
         <v>0.004423947936696039</v>
       </c>
       <c r="M51" t="n">
-        <v>179.1615060942508</v>
+        <v>179.160245834743</v>
       </c>
       <c r="N51" t="n">
         <v>0.002452435642864739</v>
       </c>
       <c r="O51" t="n">
-        <v>99.31955671253441</v>
+        <v>99.3182964530266</v>
       </c>
       <c r="P51" t="n">
         <v>40497.81968468332</v>
@@ -3636,13 +3636,13 @@
         <v>0.002485691494831069</v>
       </c>
       <c r="M52" t="n">
-        <v>134.338137300456</v>
+        <v>134.337541640328</v>
       </c>
       <c r="N52" t="n">
         <v>0.001082338208415669</v>
       </c>
       <c r="O52" t="n">
-        <v>58.49484341545506</v>
+        <v>58.4942477553271</v>
       </c>
       <c r="P52" t="n">
         <v>54044.33410971532</v>
@@ -3701,13 +3701,13 @@
         <v>0.001228066336613659</v>
       </c>
       <c r="M53" t="n">
-        <v>71.24205215734455</v>
+        <v>71.2418157261492</v>
       </c>
       <c r="N53" t="n">
         <v>0.0003861060149173587</v>
       </c>
       <c r="O53" t="n">
-        <v>22.39877692156444</v>
+        <v>22.3985404903691</v>
       </c>
       <c r="P53" t="n">
         <v>58011.37414335085</v>
@@ -3766,13 +3766,13 @@
         <v>0.004655036302394712</v>
       </c>
       <c r="M54" t="n">
-        <v>162.190358530785</v>
+        <v>162.188065728032</v>
       </c>
       <c r="N54" t="n">
         <v>0.004477101959842712</v>
       </c>
       <c r="O54" t="n">
-        <v>155.990873721128</v>
+        <v>155.988580918375</v>
       </c>
       <c r="P54" t="n">
         <v>34841.41802387166</v>
@@ -3827,13 +3827,13 @@
         <v>0.002787434520705606</v>
       </c>
       <c r="M55" t="n">
-        <v>152.3994744203073</v>
+        <v>152.399409973673</v>
       </c>
       <c r="N55" t="n">
         <v>0.0009389922022407065</v>
       </c>
       <c r="O55" t="n">
-        <v>51.33825966821714</v>
+        <v>51.3381952215828</v>
       </c>
       <c r="P55" t="n">
         <v>54673.71837495033</v>
@@ -3888,13 +3888,13 @@
         <v>0.002531234604146474</v>
       </c>
       <c r="M56" t="n">
-        <v>126.8047929170277</v>
+        <v>126.804257125663</v>
       </c>
       <c r="N56" t="n">
         <v>0.0009362218356743738</v>
       </c>
       <c r="O56" t="n">
-        <v>46.90133044036349</v>
+        <v>46.9007946489988</v>
       </c>
       <c r="P56" t="n">
         <v>50095.81368631024</v>
@@ -3953,13 +3953,13 @@
         <v>0.002571921967269722</v>
       </c>
       <c r="M57" t="n">
-        <v>149.984846787098</v>
+        <v>149.984671993292</v>
       </c>
       <c r="N57" t="n">
         <v>0.001076732829417522</v>
       </c>
       <c r="O57" t="n">
-        <v>62.79112346945066</v>
+        <v>62.7909486756447</v>
       </c>
       <c r="P57" t="n">
         <v>58316.18295655812</v>
@@ -4014,13 +4014,13 @@
         <v>0.003432602724840315</v>
       </c>
       <c r="M58" t="n">
-        <v>151.9698658975612</v>
+        <v>151.968738810775</v>
       </c>
       <c r="N58" t="n">
         <v>0.001448252989332415</v>
       </c>
       <c r="O58" t="n">
-        <v>64.11841589364063</v>
+        <v>64.1172888068544</v>
       </c>
       <c r="P58" t="n">
         <v>44272.16051279124</v>
@@ -4075,13 +4075,13 @@
         <v>0.004615041001057621</v>
       </c>
       <c r="M59" t="n">
-        <v>159.317311668464</v>
+        <v>159.315233127494</v>
       </c>
       <c r="N59" t="n">
         <v>0.004502664230031621</v>
       </c>
       <c r="O59" t="n">
-        <v>155.4379676994679</v>
+        <v>155.435889158498</v>
       </c>
       <c r="P59" t="n">
         <v>34520.87058186135</v>
@@ -4136,13 +4136,13 @@
         <v>0.002183439006668277</v>
       </c>
       <c r="M60" t="n">
-        <v>114.217133473448</v>
+        <v>114.21692709225</v>
       </c>
       <c r="N60" t="n">
         <v>0.001216178373921077</v>
       </c>
       <c r="O60" t="n">
-        <v>63.61918371057877</v>
+        <v>63.6189773293808</v>
       </c>
       <c r="P60" t="n">
         <v>52310.56454676712</v>
@@ -4201,13 +4201,13 @@
         <v>0.0009431448108916057</v>
       </c>
       <c r="M61" t="n">
-        <v>51.96723090106671</v>
+        <v>51.966869050494</v>
       </c>
       <c r="N61" t="n">
         <v>0.0005060832287942057</v>
       </c>
       <c r="O61" t="n">
-        <v>27.88532773883041</v>
+        <v>27.8849658882577</v>
       </c>
       <c r="P61" t="n">
         <v>55099.56525272816</v>
@@ -4266,13 +4266,13 @@
         <v>0.003881752702090299</v>
       </c>
       <c r="M62" t="n">
-        <v>157.455688597792</v>
+        <v>157.454775694613</v>
       </c>
       <c r="N62" t="n">
         <v>0.002624151374523599</v>
       </c>
       <c r="O62" t="n">
-        <v>106.443851898707</v>
+        <v>106.442938995528</v>
       </c>
       <c r="P62" t="n">
         <v>40562.80442848011</v>
@@ -4327,13 +4327,13 @@
         <v>0.002347687751566579</v>
       </c>
       <c r="M63" t="n">
-        <v>120.321844418785</v>
+        <v>120.321861081836</v>
       </c>
       <c r="N63" t="n">
         <v>0.001206472803963879</v>
       </c>
       <c r="O63" t="n">
-        <v>61.83318624934164</v>
+        <v>61.8332029123926</v>
       </c>
       <c r="P63" t="n">
         <v>51251.21984452443</v>
@@ -4388,13 +4388,13 @@
         <v>0.002376444629577968</v>
       </c>
       <c r="M64" t="n">
-        <v>117.9320406412402</v>
+        <v>117.932091658521</v>
       </c>
       <c r="N64" t="n">
         <v>0.0007500416501684681</v>
       </c>
       <c r="O64" t="n">
-        <v>37.2210899823665</v>
+        <v>37.2211409996473</v>
       </c>
       <c r="P64" t="n">
         <v>49625.43212271877</v>
@@ -4453,13 +4453,13 @@
         <v>0.002801238875892798</v>
       </c>
       <c r="M65" t="n">
-        <v>137.5294061384351</v>
+        <v>137.529404464271</v>
       </c>
       <c r="N65" t="n">
         <v>0.0007091321681881983</v>
       </c>
       <c r="O65" t="n">
-        <v>34.81549906593764</v>
+        <v>34.8154973917735</v>
       </c>
       <c r="P65" t="n">
         <v>49095.9216823086</v>
@@ -4518,13 +4518,13 @@
         <v>0.002836324709717948</v>
       </c>
       <c r="M66" t="n">
-        <v>125.6507290729383</v>
+        <v>125.650398590921</v>
       </c>
       <c r="N66" t="n">
         <v>0.002755051091441948</v>
       </c>
       <c r="O66" t="n">
-        <v>122.0502729981043</v>
+        <v>122.049942516087</v>
       </c>
       <c r="P66" t="n">
         <v>44300.42800121289</v>
@@ -4579,13 +4579,13 @@
         <v>0.002286106157598223</v>
       </c>
       <c r="M67" t="n">
-        <v>96.78739522297022</v>
+        <v>96.78575508036739</v>
       </c>
       <c r="N67" t="n">
         <v>0.001057175141954723</v>
       </c>
       <c r="O67" t="n">
-        <v>44.75874559293723</v>
+        <v>44.7571054503344</v>
       </c>
       <c r="P67" t="n">
         <v>42336.50950927417</v>
@@ -4640,13 +4640,13 @@
         <v>0.004985253954606032</v>
       </c>
       <c r="M68" t="n">
-        <v>165.15848855985</v>
+        <v>165.156659126179</v>
       </c>
       <c r="N68" t="n">
         <v>0.004869934368226032</v>
       </c>
       <c r="O68" t="n">
-        <v>161.338061798895</v>
+        <v>161.336232365224</v>
       </c>
       <c r="P68" t="n">
         <v>33129.03627980388</v>
@@ -4701,13 +4701,13 @@
         <v>0.004318579631240168</v>
       </c>
       <c r="M69" t="n">
-        <v>188.3592353572515</v>
+        <v>188.358407583882</v>
       </c>
       <c r="N69" t="n">
         <v>0.001009341110338468</v>
       </c>
       <c r="O69" t="n">
-        <v>44.02407163739537</v>
+        <v>44.0232438640259</v>
       </c>
       <c r="P69" t="n">
         <v>43615.8236428747</v>
@@ -4762,13 +4762,13 @@
         <v>0.004512857274977415</v>
       </c>
       <c r="M70" t="n">
-        <v>178.2473320944085</v>
+        <v>178.246468462332</v>
       </c>
       <c r="N70" t="n">
         <v>0.002002363297588115</v>
       </c>
       <c r="O70" t="n">
-        <v>79.08915839217553</v>
+        <v>79.088294760099</v>
       </c>
       <c r="P70" t="n">
         <v>39497.47523606849</v>
@@ -4827,13 +4827,13 @@
         <v>0.002394123425083844</v>
       </c>
       <c r="M71" t="n">
-        <v>89.57902472771565</v>
+        <v>89.5786348354455</v>
       </c>
       <c r="N71" t="n">
         <v>0.0007743519844788439</v>
       </c>
       <c r="O71" t="n">
-        <v>28.97358021528105</v>
+        <v>28.9731903230109</v>
       </c>
       <c r="P71" t="n">
         <v>37416.04709970556</v>
@@ -4892,13 +4892,13 @@
         <v>0.002247436524562911</v>
       </c>
       <c r="M72" t="n">
-        <v>94.78642685896079</v>
+        <v>94.7858175387026</v>
       </c>
       <c r="N72" t="n">
         <v>0.001122998209341511</v>
       </c>
       <c r="O72" t="n">
-        <v>47.36314979851969</v>
+        <v>47.3625404782615</v>
       </c>
       <c r="P72" t="n">
         <v>42175.08103243844</v>
@@ -4957,13 +4957,13 @@
         <v>0.003379981590037871</v>
       </c>
       <c r="M73" t="n">
-        <v>117.9854735511462</v>
+        <v>117.984652395155</v>
       </c>
       <c r="N73" t="n">
         <v>0.001742125797689571</v>
       </c>
       <c r="O73" t="n">
-        <v>60.81301826228763</v>
+        <v>60.8121971062964</v>
       </c>
       <c r="P73" t="n">
         <v>34906.89202062578</v>
@@ -5022,13 +5022,13 @@
         <v>0.002353998885612358</v>
       </c>
       <c r="M74" t="n">
-        <v>89.71014807334831</v>
+        <v>89.70936921435261</v>
       </c>
       <c r="N74" t="n">
         <v>0.001305101309399858</v>
       </c>
       <c r="O74" t="n">
-        <v>49.7373424328694</v>
+        <v>49.7365635738737</v>
       </c>
       <c r="P74" t="n">
         <v>38109.35075740957</v>
@@ -5087,13 +5087,13 @@
         <v>0.00086619561294452</v>
       </c>
       <c r="M75" t="n">
-        <v>46.67060984812696</v>
+        <v>46.6700725180651</v>
       </c>
       <c r="N75" t="n">
         <v>0.0004282357690355199</v>
       </c>
       <c r="O75" t="n">
-        <v>23.07361008296806</v>
+        <v>23.0730727529062</v>
       </c>
       <c r="P75" t="n">
         <v>53879.36837894645</v>
@@ -5152,13 +5152,13 @@
         <v>0.002126363259529328</v>
       </c>
       <c r="M76" t="n">
-        <v>79.62895968259609</v>
+        <v>79.6278853066987</v>
       </c>
       <c r="N76" t="n">
         <v>0.001482544388101528</v>
       </c>
       <c r="O76" t="n">
-        <v>55.51928085768599</v>
+        <v>55.5182064817886</v>
       </c>
       <c r="P76" t="n">
         <v>37447.92191543245</v>
@@ -5217,13 +5217,13 @@
         <v>0.001798177991279841</v>
       </c>
       <c r="M77" t="n">
-        <v>70.2108031923044</v>
+        <v>70.2101465114052</v>
       </c>
       <c r="N77" t="n">
         <v>0.0009939696897874406</v>
       </c>
       <c r="O77" t="n">
-        <v>38.81036177477699</v>
+        <v>38.8097050938778</v>
       </c>
       <c r="P77" t="n">
         <v>39045.15951807063</v>
@@ -5278,13 +5278,13 @@
         <v>0.002908448967036806</v>
       </c>
       <c r="M78" t="n">
-        <v>110.0829233613503</v>
+        <v>110.081902277342</v>
       </c>
       <c r="N78" t="n">
         <v>0.0004249535703063059</v>
       </c>
       <c r="O78" t="n">
-        <v>16.08509129773686</v>
+        <v>16.0840702137286</v>
       </c>
       <c r="P78" t="n">
         <v>37849.00595642768</v>
@@ -5343,13 +5343,13 @@
         <v>0.001390335852471714</v>
       </c>
       <c r="M79" t="n">
-        <v>60.0919685363724</v>
+        <v>60.0918208946391</v>
       </c>
       <c r="N79" t="n">
         <v>0.0008311687471325139</v>
       </c>
       <c r="O79" t="n">
-        <v>35.924160819639</v>
+        <v>35.9240131779057</v>
       </c>
       <c r="P79" t="n">
         <v>43221.08272458697</v>
@@ -5408,13 +5408,13 @@
         <v>0.003356995818494748</v>
       </c>
       <c r="M80" t="n">
-        <v>119.0909199183344</v>
+        <v>119.090300315133</v>
       </c>
       <c r="N80" t="n">
         <v>0.0003564904747817478</v>
       </c>
       <c r="O80" t="n">
-        <v>12.64721197229136</v>
+        <v>12.64659236909</v>
       </c>
       <c r="P80" t="n">
         <v>35475.26024876975</v>
@@ -5469,13 +5469,13 @@
         <v>0.002644959504997883</v>
       </c>
       <c r="M81" t="n">
-        <v>115.7162382385052</v>
+        <v>115.716025680978</v>
       </c>
       <c r="N81" t="n">
         <v>0.0006753540432521833</v>
       </c>
       <c r="O81" t="n">
-        <v>29.54670870049349</v>
+        <v>29.5464961429663</v>
       </c>
       <c r="P81" t="n">
         <v>43749.63981955958</v>
@@ -5530,13 +5530,13 @@
         <v>0.000916007180450091</v>
       </c>
       <c r="M82" t="n">
-        <v>43.10030926288472</v>
+        <v>43.099975477242</v>
       </c>
       <c r="N82" t="n">
         <v>0.0003289580731545218</v>
       </c>
       <c r="O82" t="n">
-        <v>15.47847106294452</v>
+        <v>15.4781372773018</v>
       </c>
       <c r="P82" t="n">
         <v>47052.00613827537</v>
@@ -5595,13 +5595,13 @@
         <v>0.001611940297469171</v>
       </c>
       <c r="M83" t="n">
-        <v>51.7862928738176</v>
+        <v>51.7861136852212</v>
       </c>
       <c r="N83" t="n">
         <v>0.0008208543378776712</v>
       </c>
       <c r="O83" t="n">
-        <v>26.3714139837567</v>
+        <v>26.3712347951603</v>
       </c>
       <c r="P83" t="n">
         <v>32126.57054763632</v>
@@ -5660,13 +5660,13 @@
         <v>0.001735194130145886</v>
       </c>
       <c r="M84" t="n">
-        <v>56.77423168040801</v>
+        <v>56.7732969744529</v>
       </c>
       <c r="N84" t="n">
         <v>0.001302955958264386</v>
       </c>
       <c r="O84" t="n">
-        <v>42.63196040966562</v>
+        <v>42.6310257037105</v>
       </c>
       <c r="P84" t="n">
         <v>32718.70045438644</v>
@@ -5725,13 +5725,13 @@
         <v>0.001133706609370434</v>
       </c>
       <c r="M85" t="n">
-        <v>56.9307150856711</v>
+        <v>56.9308587258361</v>
       </c>
       <c r="N85" t="n">
         <v>2.996225910133389e-05</v>
       </c>
       <c r="O85" t="n">
-        <v>1.504458278802527</v>
+        <v>1.50460191896753</v>
       </c>
       <c r="P85" t="n">
         <v>50216.57124981459</v>
@@ -5790,13 +5790,13 @@
         <v>0.001067499811414395</v>
       </c>
       <c r="M86" t="n">
-        <v>57.03524697731932</v>
+        <v>57.0351509504363</v>
       </c>
       <c r="N86" t="n">
         <v>0.0006235740665684951</v>
       </c>
       <c r="O86" t="n">
-        <v>33.31686164615603</v>
+        <v>33.316765619273</v>
       </c>
       <c r="P86" t="n">
         <v>53428.72227290324</v>
@@ -5855,13 +5855,13 @@
         <v>0.001197085137900995</v>
       </c>
       <c r="M87" t="n">
-        <v>51.89007595981722</v>
+        <v>51.8909929303517</v>
       </c>
       <c r="N87" t="n">
         <v>8.908567772309556e-05</v>
       </c>
       <c r="O87" t="n">
-        <v>3.860750112752852</v>
+        <v>3.86166708328733</v>
       </c>
       <c r="P87" t="n">
         <v>43347.78812920433</v>
@@ -5920,13 +5920,13 @@
         <v>0.0007068327420114108</v>
       </c>
       <c r="M88" t="n">
-        <v>43.4661887617794</v>
+        <v>43.4660299348499</v>
       </c>
       <c r="N88" t="n">
         <v>0.0004030275041435108</v>
       </c>
       <c r="O88" t="n">
-        <v>24.7839648371311</v>
+        <v>24.7838060102016</v>
       </c>
       <c r="P88" t="n">
         <v>61494.08106245905</v>
@@ -5985,13 +5985,13 @@
         <v>0.001528765867839196</v>
       </c>
       <c r="M89" t="n">
-        <v>61.76857277756732</v>
+        <v>61.7681774556576</v>
       </c>
       <c r="N89" t="n">
         <v>0.0002320617808629959</v>
       </c>
       <c r="O89" t="n">
-        <v>9.376607574268292</v>
+        <v>9.37621225235857</v>
       </c>
       <c r="P89" t="n">
         <v>40403.9485411606</v>
@@ -6050,13 +6050,13 @@
         <v>0.001342796750131465</v>
       </c>
       <c r="M90" t="n">
-        <v>56.27469490860413</v>
+        <v>56.27423602054</v>
       </c>
       <c r="N90" t="n">
         <v>0.0009467802092584651</v>
       </c>
       <c r="O90" t="n">
-        <v>39.67834234300313</v>
+        <v>39.677883454939</v>
       </c>
       <c r="P90" t="n">
         <v>41908.23072444175</v>
@@ -6111,13 +6111,13 @@
         <v>0.0007534672376625887</v>
       </c>
       <c r="M91" t="n">
-        <v>40.97033577119593</v>
+        <v>40.9703547439299</v>
       </c>
       <c r="N91" t="n">
         <v>0.0006351934706628887</v>
       </c>
       <c r="O91" t="n">
-        <v>34.53910963598793</v>
+        <v>34.5391286087219</v>
       </c>
       <c r="P91" t="n">
         <v>54375.76140805859</v>
@@ -6176,13 +6176,13 @@
         <v>0.001236940839766448</v>
       </c>
       <c r="M92" t="n">
-        <v>54.10323269412533</v>
+        <v>54.103419580053</v>
       </c>
       <c r="N92" t="n">
         <v>0.0001282871298544483</v>
       </c>
       <c r="O92" t="n">
-        <v>5.611053514661315</v>
+        <v>5.61124040058898</v>
       </c>
       <c r="P92" t="n">
         <v>43739.69865063918</v>
@@ -6237,13 +6237,13 @@
         <v>0.002307464252340363</v>
       </c>
       <c r="M93" t="n">
-        <v>66.95659507309348</v>
+        <v>66.9553327522687</v>
       </c>
       <c r="N93" t="n">
         <v>0.001651962618843763</v>
       </c>
       <c r="O93" t="n">
-        <v>47.93600572012499</v>
+        <v>47.9347433993002</v>
       </c>
       <c r="P93" t="n">
         <v>29016.84508627111</v>
@@ -6298,13 +6298,13 @@
         <v>0.000950103311477327</v>
       </c>
       <c r="M94" t="n">
-        <v>43.08654558554308</v>
+        <v>43.0868710364167</v>
       </c>
       <c r="N94" t="n">
         <v>3.835712248292705e-05</v>
       </c>
       <c r="O94" t="n">
-        <v>1.739157371452434</v>
+        <v>1.73948282232606</v>
       </c>
       <c r="P94" t="n">
         <v>45349.66936324052</v>
@@ -6363,13 +6363,13 @@
         <v>0.00131027395965521</v>
       </c>
       <c r="M95" t="n">
-        <v>59.72135790308972</v>
+        <v>59.7216564670194</v>
       </c>
       <c r="N95" t="n">
         <v>2.030809767081032e-05</v>
       </c>
       <c r="O95" t="n">
-        <v>0.9253347539407016</v>
+        <v>0.9256333178703851</v>
       </c>
       <c r="P95" t="n">
         <v>45579.5187158682</v>
@@ -6428,13 +6428,13 @@
         <v>0.0007541473740330103</v>
       </c>
       <c r="M96" t="n">
-        <v>54.06902831247294</v>
+        <v>54.0681392270688</v>
       </c>
       <c r="N96" t="n">
         <v>0.0004594203600666103</v>
       </c>
       <c r="O96" t="n">
-        <v>32.93875354947144</v>
+        <v>32.9378644640673</v>
       </c>
       <c r="P96" t="n">
         <v>71694.39434354132</v>
@@ -6493,13 +6493,13 @@
         <v>0.000948348554995344</v>
       </c>
       <c r="M97" t="n">
-        <v>41.45660575247632</v>
+        <v>41.4568277525965</v>
       </c>
       <c r="N97" t="n">
         <v>0.000656170014276044</v>
       </c>
       <c r="O97" t="n">
-        <v>28.68409149935502</v>
+        <v>28.6843134994752</v>
       </c>
       <c r="P97" t="n">
         <v>43714.75818065652</v>
@@ -6554,13 +6554,13 @@
         <v>0.001152142993344857</v>
       </c>
       <c r="M98" t="n">
-        <v>55.17400733632297</v>
+        <v>55.1712364974773</v>
       </c>
       <c r="N98" t="n">
         <v>0.0006578419678800566</v>
       </c>
       <c r="O98" t="n">
-        <v>31.50402979500116</v>
+        <v>31.5012589561555</v>
       </c>
       <c r="P98" t="n">
         <v>47885.75447332828</v>
@@ -6619,13 +6619,13 @@
         <v>0.002952844901490266</v>
       </c>
       <c r="M99" t="n">
-        <v>71.69955218050117</v>
+        <v>71.69828730701499</v>
       </c>
       <c r="N99" t="n">
         <v>0.001928083322311666</v>
       </c>
       <c r="O99" t="n">
-        <v>46.81722595738788</v>
+        <v>46.8159610839017</v>
       </c>
       <c r="P99" t="n">
         <v>24281.08813667447</v>
@@ -6680,13 +6680,13 @@
         <v>0.004018488165852548</v>
       </c>
       <c r="M100" t="n">
-        <v>77.33363319058918</v>
+        <v>77.33133438958311</v>
       </c>
       <c r="N100" t="n">
         <v>0.003915640838196349</v>
       </c>
       <c r="O100" t="n">
-        <v>75.35445078222958</v>
+        <v>75.3521519812235</v>
       </c>
       <c r="P100" t="n">
         <v>19243.88755122208</v>
@@ -6745,13 +6745,13 @@
         <v>0.002103394436134739</v>
       </c>
       <c r="M101" t="n">
-        <v>69.88165655707766</v>
+        <v>69.8810427182453</v>
       </c>
       <c r="N101" t="n">
         <v>0.001217403133788339</v>
       </c>
       <c r="O101" t="n">
-        <v>40.44638042264157</v>
+        <v>40.4457665838092</v>
       </c>
       <c r="P101" t="n">
         <v>33222.98543617944</v>

</xml_diff>

<commit_message>
Changed DataSet query so that column headings can have spaces
</commit_message>
<xml_diff>
--- a/example/info/02 foot corrected info.xlsx
+++ b/example/info/02 foot corrected info.xlsx
@@ -436,17 +436,17 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>test id</t>
+          <t>test_id</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>old filename</t>
+          <t>old_filename</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>test type</t>
+          <t>test_type</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
@@ -471,12 +471,12 @@
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>A_0 (mm)</t>
+          <t>A_0_(mm)</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>h_0 (mm)</t>
+          <t>h_0_(mm)</t>
         </is>
       </c>
       <c r="J1" s="1" t="inlineStr">
@@ -516,7 +516,7 @@
       </c>
       <c r="Q1" s="1" t="inlineStr">
         <is>
-          <t>foot correction</t>
+          <t>foot_correction</t>
         </is>
       </c>
     </row>
@@ -807,13 +807,13 @@
         <v>192.947593520996</v>
       </c>
       <c r="L6" t="n">
-        <v>0.0005903185807671863</v>
+        <v>0.0005903185807671859</v>
       </c>
       <c r="M6" t="n">
         <v>35.2190159803605</v>
       </c>
       <c r="N6" t="n">
-        <v>59661.03241166723</v>
+        <v>59661.03241166724</v>
       </c>
       <c r="O6" t="inlineStr">
         <is>
@@ -822,7 +822,7 @@
       </c>
       <c r="P6" t="inlineStr"/>
       <c r="Q6" t="n">
-        <v>-0.0004346933673407137</v>
+        <v>-0.0004346933673407142</v>
       </c>
     </row>
     <row r="7">
@@ -4855,7 +4855,7 @@
         <v>47.3625404782615</v>
       </c>
       <c r="N72" t="n">
-        <v>42175.08103243844</v>
+        <v>42175.08103243845</v>
       </c>
       <c r="O72" t="inlineStr">
         <is>
@@ -4864,7 +4864,7 @@
       </c>
       <c r="P72" t="inlineStr"/>
       <c r="Q72" t="n">
-        <v>0.0006093202581949112</v>
+        <v>0.0006093202581949108</v>
       </c>
     </row>
     <row r="73">
@@ -5703,13 +5703,13 @@
         <v>57.0351509504363</v>
       </c>
       <c r="L86" t="n">
-        <v>0.0006235740665684951</v>
+        <v>0.0006235740665684949</v>
       </c>
       <c r="M86" t="n">
         <v>33.316765619273</v>
       </c>
       <c r="N86" t="n">
-        <v>53428.72227290324</v>
+        <v>53428.72227290325</v>
       </c>
       <c r="O86" t="inlineStr">
         <is>
@@ -5718,7 +5718,7 @@
       </c>
       <c r="P86" t="inlineStr"/>
       <c r="Q86" t="n">
-        <v>9.602688302589506e-05</v>
+        <v>9.602688302589484e-05</v>
       </c>
     </row>
     <row r="87">

</xml_diff>